<commit_message>
2e version fichiers 5e1b2c72750cbdaf88639094de3476ca297c316c
</commit_message>
<xml_diff>
--- a/poc-professionnel/ig/StructureDefinition-CapaciteSavoirfaire.xlsx
+++ b/poc-professionnel/ig/StructureDefinition-CapaciteSavoirfaire.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="82">
   <si>
     <t>Property</t>
   </si>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-16T13:52:06+00:00</t>
+    <t>2025-07-17T14:35:50+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -440,7 +440,9 @@
       <c r="A5" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" t="s" s="2">
+        <v>7</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">

</xml_diff>

<commit_message>
Objets au lieu de urls + lien SavoirFaire 5b21308586e35a33ef5eeeda53ba6d18ea94ede7
</commit_message>
<xml_diff>
--- a/poc-professionnel/ig/StructureDefinition-CapaciteSavoirfaire.xlsx
+++ b/poc-professionnel/ig/StructureDefinition-CapaciteSavoirfaire.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="97">
   <si>
     <t>Property</t>
   </si>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-25T12:50:30+00:00</t>
+    <t>2025-07-29T07:08:53+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -286,6 +286,19 @@
   </si>
   <si>
     <t>SavoirFaire.dateAbandon</t>
+  </si>
+  <si>
+    <t>CapaciteSavoirfaire.exerciceProfessionnel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(https://interop.esante.gouv.fr/ig/fhir/mos/StructureDefinition/ExerciceProfessionnel)
+</t>
+  </si>
+  <si>
+    <t>Lien vers la classe ExerciceProfessionnel.</t>
+  </si>
+  <si>
+    <t>SavoirFaire.exerciceProfessionnel</t>
   </si>
   <si>
     <t>CapaciteSavoirfaire.capaciteSavoirFaire</t>
@@ -597,7 +610,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AJ6"/>
+  <dimension ref="A1:AJ7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -606,8 +619,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="33.05078125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="33.05078125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="33.953125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="33.953125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="10.8515625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="7.6796875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="5.80859375" customWidth="true" bestFit="true"/>
@@ -616,7 +629,7 @@
     <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="7.6796875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="75.46875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1164,7 +1177,7 @@
       </c>
       <c r="E6" s="2"/>
       <c r="F6" t="s" s="2">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="G6" t="s" s="2">
         <v>77</v>
@@ -1179,13 +1192,13 @@
         <v>70</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="M6" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -1212,11 +1225,13 @@
         <v>70</v>
       </c>
       <c r="X6" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="Y6" s="2"/>
+        <v>70</v>
+      </c>
+      <c r="Y6" t="s" s="2">
+        <v>70</v>
+      </c>
       <c r="Z6" t="s" s="2">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="AA6" t="s" s="2">
         <v>70</v>
@@ -1234,10 +1249,10 @@
         <v>70</v>
       </c>
       <c r="AF6" t="s" s="2">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="AG6" t="s" s="2">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="AH6" t="s" s="2">
         <v>77</v>
@@ -1246,6 +1261,104 @@
         <v>70</v>
       </c>
       <c r="AJ6" t="s" s="2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="B7" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="G7" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="H7" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="I7" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="J7" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="K7" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="L7" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="M7" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="Q7" s="2"/>
+      <c r="R7" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="S7" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="T7" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="U7" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="V7" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="W7" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="X7" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Y7" s="2"/>
+      <c r="Z7" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AA7" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="AB7" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="AC7" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="AD7" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="AE7" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="AF7" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="AG7" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AH7" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AI7" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="AJ7" t="s" s="2">
         <v>70</v>
       </c>
     </row>

</xml_diff>